<commit_message>
[Step] finish six stage proc
</commit_message>
<xml_diff>
--- a/riscv/perf.xlsx
+++ b/riscv/perf.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>TwoCycle</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>TwoStageBtb</t>
+  </si>
+  <si>
+    <t>SixStage</t>
   </si>
   <si>
     <t>Synthesis Result</t>
@@ -386,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -415,9 +418,6 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -433,7 +433,7 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -452,9 +452,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -822,15 +819,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="39" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="40" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="41" width="23.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="42" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="42" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="41" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="41" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="41" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="41" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="37" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="38" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="39" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="40" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="40" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="40" width="9.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="40" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="39" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="39" width="10.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -843,52 +840,54 @@
       <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5"/>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="I1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
+      <c r="G2" s="9"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="11"/>
+      <c r="I2" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="17"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>9</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>10</v>
       </c>
       <c r="D4" s="9">
         <v>8334</v>
@@ -902,240 +901,250 @@
       <c r="G4" s="9">
         <v>4265</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="11"/>
+      <c r="H4" s="9">
+        <v>5277</v>
+      </c>
+      <c r="I4" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="21">
+        <v>4168</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="22"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="27"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="22">
-        <v>4168</v>
-      </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="24"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26" t="s">
+      <c r="D7" s="30">
+        <v>8484</v>
+      </c>
+      <c r="E7" s="30">
+        <v>16968</v>
+      </c>
+      <c r="F7" s="30">
+        <v>5088</v>
+      </c>
+      <c r="G7" s="30">
+        <v>4880</v>
+      </c>
+      <c r="H7" s="30">
+        <v>7443</v>
+      </c>
+      <c r="I7" s="31"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="29"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="30" t="s">
+      <c r="D8" s="21">
+        <v>4243</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="22"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="32">
-        <v>8484</v>
-      </c>
-      <c r="E7" s="32">
-        <v>16968</v>
-      </c>
-      <c r="F7" s="32">
-        <v>5088</v>
-      </c>
-      <c r="G7" s="32">
-        <v>4880</v>
-      </c>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21" t="s">
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="27"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="22">
-        <v>4243</v>
-      </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="24"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="26" t="s">
+      <c r="D10" s="30">
+        <v>41784</v>
+      </c>
+      <c r="E10" s="30">
+        <v>83568</v>
+      </c>
+      <c r="F10" s="30">
+        <v>27009</v>
+      </c>
+      <c r="G10" s="30">
+        <v>21483</v>
+      </c>
+      <c r="H10" s="30">
+        <v>26383</v>
+      </c>
+      <c r="I10" s="31"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="29"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="32">
-        <v>41784</v>
-      </c>
-      <c r="E10" s="32">
-        <v>83568</v>
-      </c>
-      <c r="F10" s="32">
-        <v>27009</v>
-      </c>
-      <c r="G10" s="32">
-        <v>21483</v>
-      </c>
-      <c r="H10" s="32"/>
-      <c r="I10" s="33"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21" t="s">
+      <c r="D11" s="21">
+        <v>20893</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="22"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="27"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="29" t="s">
         <v>10</v>
-      </c>
-      <c r="D11" s="22">
-        <v>20893</v>
-      </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="24"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="29"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>9</v>
       </c>
       <c r="D13" s="9">
         <v>246990</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="30">
         <v>493980</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="30">
         <v>145938</v>
       </c>
-      <c r="G13" s="32">
+      <c r="G13" s="30">
         <v>139424</v>
       </c>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33"/>
+      <c r="H13" s="30">
+        <v>200585</v>
+      </c>
+      <c r="I13" s="31"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="21">
+        <v>123496</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="22"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="27"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="22">
-        <v>123496</v>
-      </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="24"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26" t="s">
+      <c r="D16" s="21">
+        <v>4814</v>
+      </c>
+      <c r="E16" s="21">
+        <v>9628</v>
+      </c>
+      <c r="F16" s="21">
+        <v>2708</v>
+      </c>
+      <c r="G16" s="21">
+        <v>2411</v>
+      </c>
+      <c r="H16" s="21">
+        <v>3016</v>
+      </c>
+      <c r="I16" s="22"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="29"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="22">
-        <v>4814</v>
-      </c>
-      <c r="E16" s="22">
-        <v>9628</v>
-      </c>
-      <c r="F16" s="22">
-        <v>2708</v>
-      </c>
-      <c r="G16" s="22">
-        <v>2411</v>
-      </c>
-      <c r="H16" s="22"/>
-      <c r="I16" s="24"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="22">
+      <c r="D17" s="21">
         <v>2408</v>
       </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="24"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="22"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="38"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
[Step] fix sixstage bubble after redirect
</commit_message>
<xml_diff>
--- a/riscv/perf.xlsx
+++ b/riscv/perf.xlsx
@@ -389,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -401,9 +401,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -819,18 +816,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="37" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="38" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="39" width="23.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="40" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="40" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="40" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="40" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="36" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="37" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="38" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="39" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="39" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="39" width="9.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="39" width="12.005" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="39" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="39" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="38" width="10.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -846,305 +843,305 @@
       <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="16"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>8334</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>16668</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>4342</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>4265</v>
       </c>
-      <c r="H4" s="9">
-        <v>5277</v>
-      </c>
-      <c r="I4" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20" t="s">
+      <c r="H4" s="8">
+        <v>5167</v>
+      </c>
+      <c r="I4" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="10"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="20">
         <v>4168</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="22"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24" t="s">
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="10"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="28" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="29">
         <v>8484</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="29">
         <v>16968</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="29">
         <v>5088</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="29">
         <v>4880</v>
       </c>
-      <c r="H7" s="30">
-        <v>7443</v>
-      </c>
-      <c r="I7" s="31"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20" t="s">
+      <c r="H7" s="29">
+        <v>6799</v>
+      </c>
+      <c r="I7" s="30"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="10"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="20">
         <v>4243</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="22"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="24" t="s">
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="21"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="10"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="27"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="26"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="28" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="29">
         <v>41784</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="29">
         <v>83568</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="29">
         <v>27009</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="29">
         <v>21483</v>
       </c>
-      <c r="H10" s="30">
-        <v>26383</v>
-      </c>
-      <c r="I10" s="31"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20" t="s">
+      <c r="H10" s="29">
+        <v>25620</v>
+      </c>
+      <c r="I10" s="30"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="10"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="20">
         <v>20893</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="22"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24" t="s">
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="21"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="10"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="27"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="26"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="28" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>246990</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="29">
         <v>493980</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="29">
         <v>145938</v>
       </c>
-      <c r="G13" s="30">
+      <c r="G13" s="29">
         <v>139424</v>
       </c>
-      <c r="H13" s="30">
-        <v>200585</v>
-      </c>
-      <c r="I13" s="31"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20" t="s">
+      <c r="H13" s="29">
+        <v>188590</v>
+      </c>
+      <c r="I13" s="30"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="10"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="20">
         <v>123496</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="22"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24" t="s">
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="21"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="10"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="27"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="32" t="s">
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="26"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="10"/>
+      <c r="B16" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="20">
         <v>4814</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="20">
         <v>9628</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="20">
         <v>2708</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="20">
         <v>2411</v>
       </c>
-      <c r="H16" s="21">
-        <v>3016</v>
-      </c>
-      <c r="I16" s="22"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20" t="s">
+      <c r="H16" s="20">
+        <v>3014</v>
+      </c>
+      <c r="I16" s="21"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="10"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="20">
         <v>2408</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="22"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34" t="s">
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="21"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="10"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="36"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>